<commit_message>
enhancement of public dashboard and reporting
</commit_message>
<xml_diff>
--- a/api/templates/projects_import_template.xlsx
+++ b/api/templates/projects_import_template.xlsx
@@ -58,7 +58,7 @@
     <t xml:space="preserve">Directorate</t>
   </si>
   <si>
-    <t xml:space="preserve">Sub-Count</t>
+    <t xml:space="preserve">Sub-County</t>
   </si>
   <si>
     <t xml:space="preserve">Ward</t>
@@ -167,11 +167,11 @@
   </sheetPr>
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.88"/>

</xml_diff>